<commit_message>
Run code and results with the new data
Run the code and obtain the results compare with the new HKG list
</commit_message>
<xml_diff>
--- a/Data/ENS_ID_HKG.xlsx
+++ b/Data/ENS_ID_HKG.xlsx
@@ -13,7 +13,1117 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="739">
+  <si>
+    <t>ENSG00000149313</t>
+  </si>
+  <si>
+    <t>ENSG00000100997</t>
+  </si>
+  <si>
+    <t>ENSG00000177646</t>
+  </si>
+  <si>
+    <t>ENSG00000161533</t>
+  </si>
+  <si>
+    <t>ENSG00000197894</t>
+  </si>
+  <si>
+    <t>ENSG00000182551</t>
+  </si>
+  <si>
+    <t>ENSG00000181915</t>
+  </si>
+  <si>
+    <t>ENSG00000204310</t>
+  </si>
+  <si>
+    <t>ENSG00000160216</t>
+  </si>
+  <si>
+    <t>ENSG00000101444</t>
+  </si>
+  <si>
+    <t>ENSG00000004455</t>
+  </si>
+  <si>
+    <t>ENSG00000147853</t>
+  </si>
+  <si>
+    <t>ENSG00000117448</t>
+  </si>
+  <si>
+    <t>ENSG00000053371</t>
+  </si>
+  <si>
+    <t>ENSG00000143149</t>
+  </si>
+  <si>
+    <t>ENSG00000149925</t>
+  </si>
+  <si>
+    <t>ENSG00000159461</t>
+  </si>
+  <si>
+    <t>ENSG00000141552</t>
+  </si>
+  <si>
+    <t>ENSG00000166747</t>
+  </si>
+  <si>
+    <t>ENSG00000198931</t>
+  </si>
+  <si>
+    <t>ENSG00000095139</t>
+  </si>
+  <si>
+    <t>ENSG00000116539</t>
+  </si>
+  <si>
+    <t>ENSG00000107669</t>
+  </si>
+  <si>
+    <t>ENSG00000099624</t>
+  </si>
+  <si>
+    <t>ENSG00000124172</t>
+  </si>
+  <si>
+    <t>ENSG00000159199</t>
+  </si>
+  <si>
+    <t>ENSG00000169020</t>
+  </si>
+  <si>
+    <t>ENSG00000241468</t>
+  </si>
+  <si>
+    <t>ENSG00000167283</t>
+  </si>
+  <si>
+    <t>ENSG00000167863</t>
+  </si>
+  <si>
+    <t>ENSG00000154723</t>
+  </si>
+  <si>
+    <t>ENSG00000241837</t>
+  </si>
+  <si>
+    <t>ENSG00000071553</t>
+  </si>
+  <si>
+    <t>ENSG00000117410</t>
+  </si>
+  <si>
+    <t>ENSG00000185883</t>
+  </si>
+  <si>
+    <t>ENSG00000159720</t>
+  </si>
+  <si>
+    <t>ENSG00000113732</t>
+  </si>
+  <si>
+    <t>ENSG00000147416</t>
+  </si>
+  <si>
+    <t>ENSG00000131100</t>
+  </si>
+  <si>
+    <t>ENSG00000128524</t>
+  </si>
+  <si>
+    <t>ENSG00000136888</t>
+  </si>
+  <si>
+    <t>ENSG00000158850</t>
+  </si>
+  <si>
+    <t>ENSG00000158470</t>
+  </si>
+  <si>
+    <t>ENSG00000027847</t>
+  </si>
+  <si>
+    <t>ENSG00000174684</t>
+  </si>
+  <si>
+    <t>ENSG00000185825</t>
+  </si>
+  <si>
+    <t>ENSG00000103507</t>
+  </si>
+  <si>
+    <t>ENSG00000164039</t>
+  </si>
+  <si>
+    <t>ENSG00000172331</t>
+  </si>
+  <si>
+    <t>ENSG00000198668</t>
+  </si>
+  <si>
+    <t>ENSG00000160014</t>
+  </si>
+  <si>
+    <t>ENSG00000145439</t>
+  </si>
+  <si>
+    <t>ENSG00000099804</t>
+  </si>
+  <si>
+    <t>ENSG00000103502</t>
+  </si>
+  <si>
+    <t>ENSG00000101290</t>
+  </si>
+  <si>
+    <t>ENSG00000100422</t>
+  </si>
+  <si>
+    <t>ENSG00000143418</t>
+  </si>
+  <si>
+    <t>ENSG00000111726</t>
+  </si>
+  <si>
+    <t>ENSG00000162368</t>
+  </si>
+  <si>
+    <t>ENSG00000137200</t>
+  </si>
+  <si>
+    <t>ENSG00000173786</t>
+  </si>
+  <si>
+    <t>ENSG00000068120</t>
+  </si>
+  <si>
+    <t>ENSG00000093010</t>
+  </si>
+  <si>
+    <t>ENSG00000184432</t>
+  </si>
+  <si>
+    <t>ENSG00000105669</t>
+  </si>
+  <si>
+    <t>ENSG00000181789</t>
+  </si>
+  <si>
+    <t>ENSG00000110871</t>
+  </si>
+  <si>
+    <t>ENSG00000131143</t>
+  </si>
+  <si>
+    <t>ENSG00000178741</t>
+  </si>
+  <si>
+    <t>ENSG00000135940</t>
+  </si>
+  <si>
+    <t>ENSG00000111775</t>
+  </si>
+  <si>
+    <t>ENSG00000126267</t>
+  </si>
+  <si>
+    <t>ENSG00000131174</t>
+  </si>
+  <si>
+    <t>ENSG00000127184</t>
+  </si>
+  <si>
+    <t>ENSG00000176340</t>
+  </si>
+  <si>
+    <t>ENSG00000005339</t>
+  </si>
+  <si>
+    <t>ENSG00000169826</t>
+  </si>
+  <si>
+    <t>ENSG00000133275</t>
+  </si>
+  <si>
+    <t>ENSG00000159692</t>
+  </si>
+  <si>
+    <t>ENSG00000164733</t>
+  </si>
+  <si>
+    <t>ENSG00000117984</t>
+  </si>
+  <si>
+    <t>ENSG00000101160</t>
+  </si>
+  <si>
+    <t>ENSG00000159348</t>
+  </si>
+  <si>
+    <t>ENSG00000100243</t>
+  </si>
+  <si>
+    <t>ENSG00000179091</t>
+  </si>
+  <si>
+    <t>ENSG00000129562</t>
+  </si>
+  <si>
+    <t>ENSG00000129187</t>
+  </si>
+  <si>
+    <t>ENSG00000179958</t>
+  </si>
+  <si>
+    <t>ENSG00000143753</t>
+  </si>
+  <si>
+    <t>ENSG00000095059</t>
+  </si>
+  <si>
+    <t>ENSG00000091140</t>
+  </si>
+  <si>
+    <t>ENSG00000119689</t>
+  </si>
+  <si>
+    <t>ENSG00000000419</t>
+  </si>
+  <si>
+    <t>ENSG00000179085</t>
+  </si>
+  <si>
+    <t>ENSG00000144048</t>
+  </si>
+  <si>
+    <t>ENSG00000128951</t>
+  </si>
+  <si>
+    <t>ENSG00000104823</t>
+  </si>
+  <si>
+    <t>ENSG00000156508</t>
+  </si>
+  <si>
+    <t>ENSG00000167658</t>
+  </si>
+  <si>
+    <t>ENSG00000243056</t>
+  </si>
+  <si>
+    <t>ENSG00000066322</t>
+  </si>
+  <si>
+    <t>ENSG00000074800</t>
+  </si>
+  <si>
+    <t>ENSG00000197217</t>
+  </si>
+  <si>
+    <t>ENSG00000139684</t>
+  </si>
+  <si>
+    <t>ENSG00000105379</t>
+  </si>
+  <si>
+    <t>ENSG00000116199</t>
+  </si>
+  <si>
+    <t>ENSG00000179115</t>
+  </si>
+  <si>
+    <t>ENSG00000088832</t>
+  </si>
+  <si>
+    <t>ENSG00000105701</t>
+  </si>
+  <si>
+    <t>ENSG00000141560</t>
+  </si>
+  <si>
+    <t>ENSG00000141349</t>
+  </si>
+  <si>
+    <t>ENSG00000171298</t>
+  </si>
+  <si>
+    <t>ENSG00000141429</t>
+  </si>
+  <si>
+    <t>ENSG00000178234</t>
+  </si>
+  <si>
+    <t>ENSG00000111640</t>
+  </si>
+  <si>
+    <t>ENSG00000070610</t>
+  </si>
+  <si>
+    <t>ENSG00000006007</t>
+  </si>
+  <si>
+    <t>ENSG00000119392</t>
+  </si>
+  <si>
+    <t>ENSG00000124767</t>
+  </si>
+  <si>
+    <t>ENSG00000023572</t>
+  </si>
+  <si>
+    <t>ENSG00000116906</t>
+  </si>
+  <si>
+    <t>ENSG00000197858</t>
+  </si>
+  <si>
+    <t>ENSG00000158669</t>
+  </si>
+  <si>
+    <t>ENSG00000105220</t>
+  </si>
+  <si>
+    <t>ENSG00000233276</t>
+  </si>
+  <si>
+    <t>ENSG00000167468</t>
+  </si>
+  <si>
+    <t>ENSG00000137106</t>
+  </si>
+  <si>
+    <t>ENSG00000173020</t>
+  </si>
+  <si>
+    <t>ENSG00000100983</t>
+  </si>
+  <si>
+    <t>ENSG00000197448</t>
+  </si>
+  <si>
+    <t>ENSG00000148834</t>
+  </si>
+  <si>
+    <t>ENSG00000143774</t>
+  </si>
+  <si>
+    <t>ENSG00000084754</t>
+  </si>
+  <si>
+    <t>ENSG00000063854</t>
+  </si>
+  <si>
+    <t>ENSG00000128708</t>
+  </si>
+  <si>
+    <t>ENSG00000115677</t>
+  </si>
+  <si>
+    <t>ENSG00000092148</t>
+  </si>
+  <si>
+    <t>ENSG00000146066</t>
+  </si>
+  <si>
+    <t>ENSG00000149084</t>
+  </si>
+  <si>
+    <t>ENSG00000086758</t>
+  </si>
+  <si>
+    <t>ENSG00000116237</t>
+  </si>
+  <si>
+    <t>ENSG00000101365</t>
+  </si>
+  <si>
+    <t>ENSG00000067829</t>
+  </si>
+  <si>
+    <t>ENSG00000010404</t>
+  </si>
+  <si>
+    <t>ENSG00000132376</t>
+  </si>
+  <si>
+    <t>ENSG00000068745</t>
+  </si>
+  <si>
+    <t>ENSG00000078747</t>
+  </si>
+  <si>
+    <t>ENSG00000100605</t>
+  </si>
+  <si>
+    <t>ENSG00000103510</t>
+  </si>
+  <si>
+    <t>ENSG00000025800</t>
+  </si>
+  <si>
+    <t>ENSG00000123684</t>
+  </si>
+  <si>
+    <t>ENSG00000198162</t>
+  </si>
+  <si>
+    <t>ENSG00000131844</t>
+  </si>
+  <si>
+    <t>ENSG00000146701</t>
+  </si>
+  <si>
+    <t>ENSG00000102858</t>
+  </si>
+  <si>
+    <t>ENSG00000143198</t>
+  </si>
+  <si>
+    <t>ENSG00000240972</t>
+  </si>
+  <si>
+    <t>ENSG00000133606</t>
+  </si>
+  <si>
+    <t>ENSG00000075975</t>
+  </si>
+  <si>
+    <t>ENSG00000143158</t>
+  </si>
+  <si>
+    <t>ENSG00000167862</t>
+  </si>
+  <si>
+    <t>ENSG00000039123</t>
+  </si>
+  <si>
+    <t>ENSG00000090432</t>
+  </si>
+  <si>
+    <t>ENSG00000005810</t>
+  </si>
+  <si>
+    <t>ENSG00000135372</t>
+  </si>
+  <si>
+    <t>ENSG00000070614</t>
+  </si>
+  <si>
+    <t>ENSG00000125356</t>
+  </si>
+  <si>
+    <t>ENSG00000174886</t>
+  </si>
+  <si>
+    <t>ENSG00000184752</t>
+  </si>
+  <si>
+    <t>ENSG00000131495</t>
+  </si>
+  <si>
+    <t>ENSG00000189043</t>
+  </si>
+  <si>
+    <t>ENSG00000128609</t>
+  </si>
+  <si>
+    <t>ENSG00000119421</t>
+  </si>
+  <si>
+    <t>ENSG00000004779</t>
+  </si>
+  <si>
+    <t>ENSG00000183648</t>
+  </si>
+  <si>
+    <t>ENSG00000140990</t>
+  </si>
+  <si>
+    <t>ENSG00000147123</t>
+  </si>
+  <si>
+    <t>ENSG00000090266</t>
+  </si>
+  <si>
+    <t>ENSG00000119013</t>
+  </si>
+  <si>
+    <t>ENSG00000065518</t>
+  </si>
+  <si>
+    <t>ENSG00000165264</t>
+  </si>
+  <si>
+    <t>ENSG00000099795</t>
+  </si>
+  <si>
+    <t>ENSG00000166136</t>
+  </si>
+  <si>
+    <t>ENSG00000147684</t>
+  </si>
+  <si>
+    <t>ENSG00000151366</t>
+  </si>
+  <si>
+    <t>ENSG00000213619</t>
+  </si>
+  <si>
+    <t>ENSG00000145494</t>
+  </si>
+  <si>
+    <t>ENSG00000110717</t>
+  </si>
+  <si>
+    <t>ENSG00000160194</t>
+  </si>
+  <si>
+    <t>ENSG00000204386</t>
+  </si>
+  <si>
+    <t>ENSG00000243678</t>
+  </si>
+  <si>
+    <t>ENSG00000136448</t>
+  </si>
+  <si>
+    <t>ENSG00000141279</t>
+  </si>
+  <si>
+    <t>ENSG00000076685</t>
+  </si>
+  <si>
+    <t>ENSG00000170502</t>
+  </si>
+  <si>
+    <t>ENSG00000069248</t>
+  </si>
+  <si>
+    <t>ENSG00000124789</t>
+  </si>
+  <si>
+    <t>ENSG00000139496</t>
+  </si>
+  <si>
+    <t>ENSG00000198408</t>
+  </si>
+  <si>
+    <t>ENSG00000105953</t>
+  </si>
+  <si>
+    <t>ENSG00000147162</t>
+  </si>
+  <si>
+    <t>ENSG00000068308</t>
+  </si>
+  <si>
+    <t>ENSG00000185624</t>
+  </si>
+  <si>
+    <t>ENSG00000007168</t>
+  </si>
+  <si>
+    <t>ENSG00000168092</t>
+  </si>
+  <si>
+    <t>ENSG00000120137</t>
+  </si>
+  <si>
+    <t>ENSG00000090060</t>
+  </si>
+  <si>
+    <t>ENSG00000143799</t>
+  </si>
+  <si>
+    <t>ENSG00000166228</t>
+  </si>
+  <si>
+    <t>ENSG00000120265</t>
+  </si>
+  <si>
+    <t>ENSG00000116005</t>
+  </si>
+  <si>
+    <t>ENSG00000161217</t>
+  </si>
+  <si>
+    <t>ENSG00000131828</t>
+  </si>
+  <si>
+    <t>ENSG00000167004</t>
+  </si>
+  <si>
+    <t>ENSG00000143870</t>
+  </si>
+  <si>
+    <t>ENSG00000141959</t>
+  </si>
+  <si>
+    <t>ENSG00000171314</t>
+  </si>
+  <si>
+    <t>ENSG00000130313</t>
+  </si>
+  <si>
+    <t>ENSG00000155252</t>
+  </si>
+  <si>
+    <t>ENSG00000100564</t>
+  </si>
+  <si>
+    <t>ENSG00000127445</t>
+  </si>
+  <si>
+    <t>ENSG00000102309</t>
+  </si>
+  <si>
+    <t>ENSG00000165782</t>
+  </si>
+  <si>
+    <t>ENSG00000186111</t>
+  </si>
+  <si>
+    <t>ENSG00000103066</t>
+  </si>
+  <si>
+    <t>ENSG00000124181</t>
+  </si>
+  <si>
+    <t>ENSG00000083444</t>
+  </si>
+  <si>
+    <t>ENSG00000106397</t>
+  </si>
+  <si>
+    <t>ENSG00000100417</t>
+  </si>
+  <si>
+    <t>ENSG00000165688</t>
+  </si>
+  <si>
+    <t>ENSG00000163344</t>
+  </si>
+  <si>
+    <t>ENSG00000106628</t>
+  </si>
+  <si>
+    <t>ENSG00000148229</t>
+  </si>
+  <si>
+    <t>ENSG00000186184</t>
+  </si>
+  <si>
+    <t>ENSG00000137054</t>
+  </si>
+  <si>
+    <t>ENSG00000102978</t>
+  </si>
+  <si>
+    <t>ENSG00000100142</t>
+  </si>
+  <si>
+    <t>ENSG00000105258</t>
+  </si>
+  <si>
+    <t>ENSG00000005075</t>
+  </si>
+  <si>
+    <t>ENSG00000147669</t>
+  </si>
+  <si>
+    <t>ENSG00000177700</t>
+  </si>
+  <si>
+    <t>ENSG00000186141</t>
+  </si>
+  <si>
+    <t>ENSG00000121851</t>
+  </si>
+  <si>
+    <t>ENSG00000085998</t>
+  </si>
+  <si>
+    <t>ENSG00000180817</t>
+  </si>
+  <si>
+    <t>ENSG00000196262</t>
+  </si>
+  <si>
+    <t>ENSG00000166794</t>
+  </si>
+  <si>
+    <t>ENSG00000171497</t>
+  </si>
+  <si>
+    <t>ENSG00000171960</t>
+  </si>
+  <si>
+    <t>ENSG00000131013</t>
+  </si>
+  <si>
+    <t>ENSG00000131238</t>
+  </si>
+  <si>
+    <t>ENSG00000117450</t>
+  </si>
+  <si>
+    <t>ENSG00000167815</t>
+  </si>
+  <si>
+    <t>ENSG00000126432</t>
+  </si>
+  <si>
+    <t>ENSG00000117592</t>
+  </si>
+  <si>
+    <t>ENSG00000085377</t>
+  </si>
+  <si>
+    <t>ENSG00000147224</t>
+  </si>
+  <si>
+    <t>ENSG00000197746</t>
+  </si>
+  <si>
+    <t>ENSG00000174915</t>
+  </si>
+  <si>
+    <t>ENSG00000171862</t>
+  </si>
+  <si>
+    <t>ENSG00000148334</t>
+  </si>
+  <si>
+    <t>ENSG00000110958</t>
+  </si>
+  <si>
+    <t>ENSG00000141378</t>
+  </si>
+  <si>
+    <t>ENSG00000143811</t>
+  </si>
+  <si>
+    <t>ENSG00000145337</t>
+  </si>
+  <si>
+    <t>ENSG00000017797</t>
+  </si>
+  <si>
+    <t>ENSG00000153201</t>
+  </si>
+  <si>
+    <t>ENSG00000240857</t>
+  </si>
+  <si>
+    <t>ENSG00000204227</t>
+  </si>
+  <si>
+    <t>ENSG00000070423</t>
+  </si>
+  <si>
+    <t>ENSG00000082996</t>
+  </si>
+  <si>
+    <t>ENSG00000170881</t>
+  </si>
+  <si>
+    <t>ENSG00000163162</t>
+  </si>
+  <si>
+    <t>ENSG00000108523</t>
+  </si>
+  <si>
+    <t>ENSG00000168159</t>
+  </si>
+  <si>
+    <t>ENSG00000034677</t>
+  </si>
+  <si>
+    <t>ENSG00000155827</t>
+  </si>
+  <si>
+    <t>ENSG00000011275</t>
+  </si>
+  <si>
+    <t>ENSG00000153574</t>
+  </si>
+  <si>
+    <t>ENSG00000241343</t>
+  </si>
+  <si>
+    <t>ENSG00000163902</t>
+  </si>
+  <si>
+    <t>ENSG00000118705</t>
+  </si>
+  <si>
+    <t>ENSG00000117118</t>
+  </si>
+  <si>
+    <t>ENSG00000204370</t>
+  </si>
+  <si>
+    <t>ENSG00000140612</t>
+  </si>
+  <si>
+    <t>ENSG00000157020</t>
+  </si>
+  <si>
+    <t>ENSG00000086475</t>
+  </si>
+  <si>
+    <t>ENSG00000099381</t>
+  </si>
+  <si>
+    <t>ENSG00000139718</t>
+  </si>
+  <si>
+    <t>ENSG00000168137</t>
+  </si>
+  <si>
+    <t>ENSG00000097033</t>
+  </si>
+  <si>
+    <t>ENSG00000181788</t>
+  </si>
+  <si>
+    <t>ENSG00000068903</t>
+  </si>
+  <si>
+    <t>ENSG00000108528</t>
+  </si>
+  <si>
+    <t>ENSG00000155287</t>
+  </si>
+  <si>
+    <t>ENSG00000075415</t>
+  </si>
+  <si>
+    <t>ENSG00000144659</t>
+  </si>
+  <si>
+    <t>ENSG00000005022</t>
+  </si>
+  <si>
+    <t>ENSG00000169100</t>
+  </si>
+  <si>
+    <t>ENSG00000164414</t>
+  </si>
+  <si>
+    <t>ENSG00000134294</t>
+  </si>
+  <si>
+    <t>ENSG00000143570</t>
+  </si>
+  <si>
+    <t>ENSG00000141424</t>
+  </si>
+  <si>
+    <t>ENSG00000112473</t>
+  </si>
+  <si>
+    <t>ENSG00000166311</t>
+  </si>
+  <si>
+    <t>ENSG00000198742</t>
+  </si>
+  <si>
+    <t>ENSG00000142168</t>
+  </si>
+  <si>
+    <t>ENSG00000118363</t>
+  </si>
+  <si>
+    <t>ENSG00000129128</t>
+  </si>
+  <si>
+    <t>ENSG00000116649</t>
+  </si>
+  <si>
+    <t>ENSG00000163527</t>
+  </si>
+  <si>
+    <t>ENSG00000103266</t>
+  </si>
+  <si>
+    <t>ENSG00000273841</t>
+  </si>
+  <si>
+    <t>ENSG00000177156</t>
+  </si>
+  <si>
+    <t>ENSG00000105254</t>
+  </si>
+  <si>
+    <t>ENSG00000112941</t>
+  </si>
+  <si>
+    <t>ENSG00000166479</t>
+  </si>
+  <si>
+    <t>ENSG00000173273</t>
+  </si>
+  <si>
+    <t>ENSG00000107854</t>
+  </si>
+  <si>
+    <t>ENSG00000111669</t>
+  </si>
+  <si>
+    <t>ENSG00000166340</t>
+  </si>
+  <si>
+    <t>ENSG00000047410</t>
+  </si>
+  <si>
+    <t>ENSG00000131653</t>
+  </si>
+  <si>
+    <t>ENSG00000153827</t>
+  </si>
+  <si>
+    <t>ENSG00000149016</t>
+  </si>
+  <si>
+    <t>ENSG00000100348</t>
+  </si>
+  <si>
+    <t>ENSG00000130985</t>
+  </si>
+  <si>
+    <t>ENSG00000126261</t>
+  </si>
+  <si>
+    <t>ENSG00000077721</t>
+  </si>
+  <si>
+    <t>ENSG00000119048</t>
+  </si>
+  <si>
+    <t>ENSG00000131508</t>
+  </si>
+  <si>
+    <t>ENSG00000109332</t>
+  </si>
+  <si>
+    <t>ENSG00000184182</t>
+  </si>
+  <si>
+    <t>ENSG00000132388</t>
+  </si>
+  <si>
+    <t>ENSG00000184787</t>
+  </si>
+  <si>
+    <t>ENSG00000186591</t>
+  </si>
+  <si>
+    <t>ENSG00000103275</t>
+  </si>
+  <si>
+    <t>ENSG00000198833</t>
+  </si>
+  <si>
+    <t>ENSG00000078140</t>
+  </si>
+  <si>
+    <t>ENSG00000185651</t>
+  </si>
+  <si>
+    <t>ENSG00000130725</t>
+  </si>
+  <si>
+    <t>ENSG00000175931</t>
+  </si>
+  <si>
+    <t>ENSG00000160714</t>
+  </si>
+  <si>
+    <t>ENSG00000107341</t>
+  </si>
+  <si>
+    <t>ENSG00000159202</t>
+  </si>
+  <si>
+    <t>ENSG00000009335</t>
+  </si>
+  <si>
+    <t>ENSG00000127481</t>
+  </si>
+  <si>
+    <t>ENSG00000169764</t>
+  </si>
+  <si>
+    <t>ENSG00000184076</t>
+  </si>
+  <si>
+    <t>ENSG00000127540</t>
+  </si>
+  <si>
+    <t>ENSG00000156467</t>
+  </si>
+  <si>
+    <t>ENSG00000173660</t>
+  </si>
+  <si>
+    <t>ENSG00000164405</t>
+  </si>
+  <si>
+    <t>ENSG00000126088</t>
+  </si>
+  <si>
+    <t>ENSG00000102226</t>
+  </si>
+  <si>
+    <t>ENSG00000152484</t>
+  </si>
+  <si>
+    <t>ENSG00000101557</t>
+  </si>
+  <si>
+    <t>ENSG00000124422</t>
+  </si>
+  <si>
+    <t>ENSG00000115464</t>
+  </si>
+  <si>
+    <t>ENSG00000114316</t>
+  </si>
+  <si>
+    <t>ENSG00000090686</t>
+  </si>
+  <si>
+    <t>ENSG00000187555</t>
+  </si>
+  <si>
+    <t>ENSG00000124486</t>
+  </si>
+  <si>
+    <t>ENSG00000167397</t>
+  </si>
+  <si>
+    <t>ENSG00000111237</t>
+  </si>
+  <si>
+    <t>ENSG00000106636</t>
+  </si>
+  <si>
+    <t>ENSG00000023041</t>
+  </si>
+  <si>
+    <t>ENSG00000153786</t>
+  </si>
+  <si>
+    <t>ENSG00000084073</t>
+  </si>
+  <si>
+    <t>ENSEMBL_ID</t>
+  </si>
   <si>
     <t>ENSG00000149313</t>
   </si>
@@ -1165,7 +2275,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A369"/>
+  <dimension ref="A1:A370"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.62109375" customWidth="true"/>
@@ -1173,1847 +2283,1852 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>0</v>
+        <v>369</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>1</v>
+        <v>370</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>2</v>
+        <v>371</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>3</v>
+        <v>372</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>4</v>
+        <v>373</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>5</v>
+        <v>374</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>6</v>
+        <v>375</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>7</v>
+        <v>376</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>8</v>
+        <v>377</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>9</v>
+        <v>378</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>10</v>
+        <v>379</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>11</v>
+        <v>380</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>12</v>
+        <v>381</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>13</v>
+        <v>382</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>14</v>
+        <v>383</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>15</v>
+        <v>384</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="s">
-        <v>16</v>
+        <v>385</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="s">
-        <v>17</v>
+        <v>386</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="s">
-        <v>18</v>
+        <v>387</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="s">
-        <v>19</v>
+        <v>388</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="s">
-        <v>20</v>
+        <v>389</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="s">
-        <v>21</v>
+        <v>390</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="s">
-        <v>22</v>
+        <v>391</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="s">
-        <v>23</v>
+        <v>392</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="s">
-        <v>24</v>
+        <v>393</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="s">
-        <v>25</v>
+        <v>394</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="s">
-        <v>26</v>
+        <v>395</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="s">
-        <v>27</v>
+        <v>396</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0" t="s">
-        <v>28</v>
+        <v>397</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="s">
-        <v>29</v>
+        <v>398</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="s">
-        <v>30</v>
+        <v>399</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="s">
-        <v>31</v>
+        <v>400</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0" t="s">
-        <v>32</v>
+        <v>401</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0" t="s">
-        <v>33</v>
+        <v>402</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0" t="s">
-        <v>34</v>
+        <v>403</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0" t="s">
-        <v>35</v>
+        <v>404</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0" t="s">
-        <v>36</v>
+        <v>405</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0" t="s">
-        <v>37</v>
+        <v>406</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0" t="s">
-        <v>38</v>
+        <v>407</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0" t="s">
-        <v>39</v>
+        <v>408</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0" t="s">
-        <v>40</v>
+        <v>409</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0" t="s">
-        <v>41</v>
+        <v>410</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0" t="s">
-        <v>42</v>
+        <v>411</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0" t="s">
-        <v>43</v>
+        <v>412</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0" t="s">
-        <v>44</v>
+        <v>413</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0" t="s">
-        <v>45</v>
+        <v>414</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0" t="s">
-        <v>46</v>
+        <v>415</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0" t="s">
-        <v>47</v>
+        <v>416</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0" t="s">
-        <v>48</v>
+        <v>417</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0" t="s">
-        <v>49</v>
+        <v>418</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0" t="s">
-        <v>50</v>
+        <v>419</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0" t="s">
-        <v>51</v>
+        <v>420</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0" t="s">
-        <v>52</v>
+        <v>421</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0" t="s">
-        <v>53</v>
+        <v>422</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0" t="s">
-        <v>54</v>
+        <v>423</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0" t="s">
-        <v>55</v>
+        <v>424</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0" t="s">
-        <v>56</v>
+        <v>425</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0" t="s">
-        <v>57</v>
+        <v>426</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0" t="s">
-        <v>58</v>
+        <v>427</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0" t="s">
-        <v>59</v>
+        <v>428</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="0" t="s">
-        <v>60</v>
+        <v>429</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="0" t="s">
-        <v>61</v>
+        <v>430</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="0" t="s">
-        <v>62</v>
+        <v>431</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="0" t="s">
-        <v>63</v>
+        <v>432</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="0" t="s">
-        <v>64</v>
+        <v>433</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="0" t="s">
-        <v>65</v>
+        <v>434</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="0" t="s">
-        <v>66</v>
+        <v>435</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="0" t="s">
-        <v>67</v>
+        <v>436</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="0" t="s">
-        <v>68</v>
+        <v>437</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="0" t="s">
-        <v>69</v>
+        <v>438</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="0" t="s">
-        <v>70</v>
+        <v>439</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="0" t="s">
-        <v>71</v>
+        <v>440</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="0" t="s">
-        <v>72</v>
+        <v>441</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="0" t="s">
-        <v>73</v>
+        <v>442</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="0" t="s">
-        <v>74</v>
+        <v>443</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="0" t="s">
-        <v>75</v>
+        <v>444</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="0" t="s">
-        <v>76</v>
+        <v>445</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="0" t="s">
-        <v>77</v>
+        <v>446</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="0" t="s">
-        <v>78</v>
+        <v>447</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="0" t="s">
-        <v>79</v>
+        <v>448</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="0" t="s">
-        <v>80</v>
+        <v>449</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="0" t="s">
-        <v>81</v>
+        <v>450</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="0" t="s">
-        <v>82</v>
+        <v>451</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="0" t="s">
-        <v>83</v>
+        <v>452</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="0" t="s">
-        <v>84</v>
+        <v>453</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="0" t="s">
-        <v>85</v>
+        <v>454</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="0" t="s">
-        <v>86</v>
+        <v>455</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="0" t="s">
-        <v>87</v>
+        <v>456</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="0" t="s">
-        <v>88</v>
+        <v>457</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="0" t="s">
-        <v>89</v>
+        <v>458</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="0" t="s">
-        <v>90</v>
+        <v>459</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="0" t="s">
-        <v>91</v>
+        <v>460</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="0" t="s">
-        <v>92</v>
+        <v>461</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="0" t="s">
-        <v>93</v>
+        <v>462</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="0" t="s">
-        <v>94</v>
+        <v>463</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="0" t="s">
-        <v>95</v>
+        <v>464</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="0" t="s">
-        <v>96</v>
+        <v>465</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="0" t="s">
-        <v>97</v>
+        <v>466</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="0" t="s">
-        <v>98</v>
+        <v>467</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="0" t="s">
-        <v>99</v>
+        <v>468</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="0" t="s">
-        <v>100</v>
+        <v>469</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="0" t="s">
-        <v>101</v>
+        <v>470</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="0" t="s">
-        <v>102</v>
+        <v>471</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="0" t="s">
-        <v>103</v>
+        <v>472</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="0" t="s">
-        <v>104</v>
+        <v>473</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="0" t="s">
-        <v>105</v>
+        <v>474</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="0" t="s">
-        <v>106</v>
+        <v>475</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="0" t="s">
-        <v>107</v>
+        <v>476</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="0" t="s">
-        <v>108</v>
+        <v>477</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="0" t="s">
-        <v>109</v>
+        <v>478</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="0" t="s">
-        <v>110</v>
+        <v>479</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="0" t="s">
-        <v>111</v>
+        <v>480</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="0" t="s">
-        <v>112</v>
+        <v>481</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="0" t="s">
-        <v>113</v>
+        <v>482</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="0" t="s">
-        <v>114</v>
+        <v>483</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="0" t="s">
-        <v>115</v>
+        <v>484</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="0" t="s">
-        <v>116</v>
+        <v>485</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="0" t="s">
-        <v>117</v>
+        <v>486</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="0" t="s">
-        <v>118</v>
+        <v>487</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="0" t="s">
-        <v>119</v>
+        <v>488</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="0" t="s">
-        <v>120</v>
+        <v>489</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="0" t="s">
-        <v>121</v>
+        <v>490</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="0" t="s">
-        <v>122</v>
+        <v>491</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="0" t="s">
-        <v>123</v>
+        <v>492</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="0" t="s">
-        <v>124</v>
+        <v>493</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="0" t="s">
-        <v>125</v>
+        <v>494</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="0" t="s">
-        <v>126</v>
+        <v>495</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="0" t="s">
-        <v>127</v>
+        <v>496</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="0" t="s">
-        <v>128</v>
+        <v>497</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="0" t="s">
-        <v>129</v>
+        <v>498</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="0" t="s">
-        <v>130</v>
+        <v>499</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="0" t="s">
-        <v>131</v>
+        <v>500</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="0" t="s">
-        <v>132</v>
+        <v>501</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="0" t="s">
-        <v>133</v>
+        <v>502</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="0" t="s">
-        <v>134</v>
+        <v>503</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="0" t="s">
-        <v>135</v>
+        <v>504</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="0" t="s">
-        <v>136</v>
+        <v>505</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="0" t="s">
-        <v>137</v>
+        <v>506</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="0" t="s">
-        <v>138</v>
+        <v>507</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="0" t="s">
-        <v>139</v>
+        <v>508</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="0" t="s">
-        <v>140</v>
+        <v>509</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="0" t="s">
-        <v>141</v>
+        <v>510</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="0" t="s">
-        <v>142</v>
+        <v>511</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="0" t="s">
-        <v>143</v>
+        <v>512</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="0" t="s">
-        <v>144</v>
+        <v>513</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="0" t="s">
-        <v>145</v>
+        <v>514</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="0" t="s">
-        <v>146</v>
+        <v>515</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="0" t="s">
-        <v>147</v>
+        <v>516</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="0" t="s">
-        <v>148</v>
+        <v>517</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="0" t="s">
-        <v>149</v>
+        <v>518</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="0" t="s">
-        <v>150</v>
+        <v>519</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="0" t="s">
-        <v>151</v>
+        <v>520</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="0" t="s">
-        <v>152</v>
+        <v>521</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="0" t="s">
-        <v>153</v>
+        <v>522</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="0" t="s">
-        <v>154</v>
+        <v>523</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="0" t="s">
-        <v>155</v>
+        <v>524</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="0" t="s">
-        <v>156</v>
+        <v>525</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="0" t="s">
-        <v>157</v>
+        <v>526</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="0" t="s">
-        <v>158</v>
+        <v>527</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="0" t="s">
-        <v>159</v>
+        <v>528</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="0" t="s">
-        <v>160</v>
+        <v>529</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="0" t="s">
-        <v>161</v>
+        <v>530</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="0" t="s">
-        <v>162</v>
+        <v>531</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="0" t="s">
-        <v>163</v>
+        <v>532</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="0" t="s">
-        <v>164</v>
+        <v>533</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="0" t="s">
-        <v>165</v>
+        <v>534</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="0" t="s">
-        <v>166</v>
+        <v>535</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="0" t="s">
-        <v>167</v>
+        <v>536</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="0" t="s">
-        <v>168</v>
+        <v>537</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="0" t="s">
-        <v>169</v>
+        <v>538</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="0" t="s">
-        <v>170</v>
+        <v>539</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="0" t="s">
-        <v>171</v>
+        <v>540</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="0" t="s">
-        <v>172</v>
+        <v>541</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="0" t="s">
-        <v>173</v>
+        <v>542</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="0" t="s">
-        <v>174</v>
+        <v>543</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="0" t="s">
-        <v>175</v>
+        <v>544</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="0" t="s">
-        <v>176</v>
+        <v>545</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="0" t="s">
-        <v>177</v>
+        <v>546</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="0" t="s">
-        <v>178</v>
+        <v>547</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="0" t="s">
-        <v>179</v>
+        <v>548</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="0" t="s">
-        <v>180</v>
+        <v>549</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="0" t="s">
-        <v>181</v>
+        <v>550</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="0" t="s">
-        <v>182</v>
+        <v>551</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="0" t="s">
-        <v>183</v>
+        <v>552</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="0" t="s">
-        <v>184</v>
+        <v>553</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="0" t="s">
-        <v>185</v>
+        <v>554</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="0" t="s">
-        <v>186</v>
+        <v>555</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="0" t="s">
-        <v>187</v>
+        <v>556</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="0" t="s">
-        <v>188</v>
+        <v>557</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="0" t="s">
-        <v>189</v>
+        <v>558</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="0" t="s">
-        <v>190</v>
+        <v>559</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="0" t="s">
-        <v>191</v>
+        <v>560</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="0" t="s">
-        <v>192</v>
+        <v>561</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="0" t="s">
-        <v>193</v>
+        <v>562</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="0" t="s">
-        <v>194</v>
+        <v>563</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="0" t="s">
-        <v>195</v>
+        <v>564</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="0" t="s">
-        <v>196</v>
+        <v>565</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="0" t="s">
-        <v>197</v>
+        <v>566</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="0" t="s">
-        <v>198</v>
+        <v>567</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="0" t="s">
-        <v>199</v>
+        <v>568</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="0" t="s">
-        <v>200</v>
+        <v>569</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="0" t="s">
-        <v>201</v>
+        <v>570</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="0" t="s">
-        <v>202</v>
+        <v>571</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="0" t="s">
-        <v>203</v>
+        <v>572</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="0" t="s">
-        <v>204</v>
+        <v>573</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="0" t="s">
-        <v>205</v>
+        <v>574</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="0" t="s">
-        <v>206</v>
+        <v>575</v>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="0" t="s">
-        <v>207</v>
+        <v>576</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="0" t="s">
-        <v>208</v>
+        <v>577</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="0" t="s">
-        <v>209</v>
+        <v>578</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="0" t="s">
-        <v>210</v>
+        <v>579</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="0" t="s">
-        <v>211</v>
+        <v>580</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="0" t="s">
-        <v>212</v>
+        <v>581</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="0" t="s">
-        <v>213</v>
+        <v>582</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="0" t="s">
-        <v>214</v>
+        <v>583</v>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="0" t="s">
-        <v>215</v>
+        <v>584</v>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="0" t="s">
-        <v>216</v>
+        <v>585</v>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="0" t="s">
-        <v>217</v>
+        <v>586</v>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="0" t="s">
-        <v>218</v>
+        <v>587</v>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="0" t="s">
-        <v>219</v>
+        <v>588</v>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="0" t="s">
-        <v>220</v>
+        <v>589</v>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="0" t="s">
-        <v>221</v>
+        <v>590</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="0" t="s">
-        <v>222</v>
+        <v>591</v>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="0" t="s">
-        <v>223</v>
+        <v>592</v>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="0" t="s">
-        <v>224</v>
+        <v>593</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="0" t="s">
-        <v>225</v>
+        <v>594</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="0" t="s">
-        <v>226</v>
+        <v>595</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="0" t="s">
-        <v>227</v>
+        <v>596</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="0" t="s">
-        <v>228</v>
+        <v>597</v>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="0" t="s">
-        <v>229</v>
+        <v>598</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="0" t="s">
-        <v>230</v>
+        <v>599</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="0" t="s">
-        <v>231</v>
+        <v>600</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="0" t="s">
-        <v>232</v>
+        <v>601</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="0" t="s">
-        <v>233</v>
+        <v>602</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="0" t="s">
-        <v>234</v>
+        <v>603</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="0" t="s">
-        <v>235</v>
+        <v>604</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="0" t="s">
-        <v>236</v>
+        <v>605</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="0" t="s">
-        <v>237</v>
+        <v>606</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="0" t="s">
-        <v>238</v>
+        <v>607</v>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="0" t="s">
-        <v>239</v>
+        <v>608</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="0" t="s">
-        <v>240</v>
+        <v>609</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="0" t="s">
-        <v>241</v>
+        <v>610</v>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="0" t="s">
-        <v>242</v>
+        <v>611</v>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="0" t="s">
-        <v>243</v>
+        <v>612</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="0" t="s">
-        <v>244</v>
+        <v>613</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="0" t="s">
-        <v>245</v>
+        <v>614</v>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="0" t="s">
-        <v>246</v>
+        <v>615</v>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="0" t="s">
-        <v>247</v>
+        <v>616</v>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="0" t="s">
-        <v>248</v>
+        <v>617</v>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="0" t="s">
-        <v>249</v>
+        <v>618</v>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="0" t="s">
-        <v>250</v>
+        <v>619</v>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="0" t="s">
-        <v>251</v>
+        <v>620</v>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="0" t="s">
-        <v>252</v>
+        <v>621</v>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="0" t="s">
-        <v>253</v>
+        <v>622</v>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="0" t="s">
-        <v>254</v>
+        <v>623</v>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="0" t="s">
-        <v>255</v>
+        <v>624</v>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="0" t="s">
-        <v>256</v>
+        <v>625</v>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="0" t="s">
-        <v>257</v>
+        <v>626</v>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="0" t="s">
-        <v>258</v>
+        <v>627</v>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="0" t="s">
-        <v>259</v>
+        <v>628</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="0" t="s">
-        <v>260</v>
+        <v>629</v>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="0" t="s">
-        <v>261</v>
+        <v>630</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="0" t="s">
-        <v>262</v>
+        <v>631</v>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="0" t="s">
-        <v>263</v>
+        <v>632</v>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="0" t="s">
-        <v>264</v>
+        <v>633</v>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="0" t="s">
-        <v>265</v>
+        <v>634</v>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="0" t="s">
-        <v>266</v>
+        <v>635</v>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="0" t="s">
-        <v>267</v>
+        <v>636</v>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="0" t="s">
-        <v>268</v>
+        <v>637</v>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="0" t="s">
-        <v>269</v>
+        <v>638</v>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="0" t="s">
-        <v>270</v>
+        <v>639</v>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="0" t="s">
-        <v>271</v>
+        <v>640</v>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="0" t="s">
-        <v>272</v>
+        <v>641</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="0" t="s">
-        <v>273</v>
+        <v>642</v>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="0" t="s">
-        <v>274</v>
+        <v>643</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="0" t="s">
-        <v>275</v>
+        <v>644</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="0" t="s">
-        <v>276</v>
+        <v>645</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="0" t="s">
-        <v>277</v>
+        <v>646</v>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="0" t="s">
-        <v>278</v>
+        <v>647</v>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="0" t="s">
-        <v>279</v>
+        <v>648</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="0" t="s">
-        <v>280</v>
+        <v>649</v>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="0" t="s">
-        <v>281</v>
+        <v>650</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="0" t="s">
-        <v>282</v>
+        <v>651</v>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="0" t="s">
-        <v>283</v>
+        <v>652</v>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="0" t="s">
-        <v>284</v>
+        <v>653</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="0" t="s">
-        <v>285</v>
+        <v>654</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="0" t="s">
-        <v>286</v>
+        <v>655</v>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="0" t="s">
-        <v>287</v>
+        <v>656</v>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="0" t="s">
-        <v>288</v>
+        <v>657</v>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="0" t="s">
-        <v>289</v>
+        <v>658</v>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="0" t="s">
-        <v>290</v>
+        <v>659</v>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="0" t="s">
-        <v>291</v>
+        <v>660</v>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="0" t="s">
-        <v>292</v>
+        <v>661</v>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="0" t="s">
-        <v>293</v>
+        <v>662</v>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="0" t="s">
-        <v>294</v>
+        <v>663</v>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="0" t="s">
-        <v>295</v>
+        <v>664</v>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="0" t="s">
-        <v>296</v>
+        <v>665</v>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="0" t="s">
-        <v>297</v>
+        <v>666</v>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="0" t="s">
-        <v>298</v>
+        <v>667</v>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="0" t="s">
-        <v>299</v>
+        <v>668</v>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="0" t="s">
-        <v>300</v>
+        <v>669</v>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="0" t="s">
-        <v>301</v>
+        <v>670</v>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="0" t="s">
-        <v>302</v>
+        <v>671</v>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="0" t="s">
-        <v>303</v>
+        <v>672</v>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="0" t="s">
-        <v>304</v>
+        <v>673</v>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="0" t="s">
-        <v>305</v>
+        <v>674</v>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="0" t="s">
-        <v>306</v>
+        <v>675</v>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="0" t="s">
-        <v>307</v>
+        <v>676</v>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="0" t="s">
-        <v>308</v>
+        <v>677</v>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="0" t="s">
-        <v>309</v>
+        <v>678</v>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="0" t="s">
-        <v>310</v>
+        <v>679</v>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="0" t="s">
-        <v>311</v>
+        <v>680</v>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="0" t="s">
-        <v>312</v>
+        <v>681</v>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="0" t="s">
-        <v>313</v>
+        <v>682</v>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="0" t="s">
-        <v>314</v>
+        <v>683</v>
       </c>
     </row>
     <row r="316">
       <c r="A316" s="0" t="s">
-        <v>315</v>
+        <v>684</v>
       </c>
     </row>
     <row r="317">
       <c r="A317" s="0" t="s">
-        <v>316</v>
+        <v>685</v>
       </c>
     </row>
     <row r="318">
       <c r="A318" s="0" t="s">
-        <v>317</v>
+        <v>686</v>
       </c>
     </row>
     <row r="319">
       <c r="A319" s="0" t="s">
-        <v>318</v>
+        <v>687</v>
       </c>
     </row>
     <row r="320">
       <c r="A320" s="0" t="s">
-        <v>319</v>
+        <v>688</v>
       </c>
     </row>
     <row r="321">
       <c r="A321" s="0" t="s">
-        <v>320</v>
+        <v>689</v>
       </c>
     </row>
     <row r="322">
       <c r="A322" s="0" t="s">
-        <v>321</v>
+        <v>690</v>
       </c>
     </row>
     <row r="323">
       <c r="A323" s="0" t="s">
-        <v>322</v>
+        <v>691</v>
       </c>
     </row>
     <row r="324">
       <c r="A324" s="0" t="s">
-        <v>323</v>
+        <v>692</v>
       </c>
     </row>
     <row r="325">
       <c r="A325" s="0" t="s">
-        <v>324</v>
+        <v>693</v>
       </c>
     </row>
     <row r="326">
       <c r="A326" s="0" t="s">
-        <v>325</v>
+        <v>694</v>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="0" t="s">
-        <v>326</v>
+        <v>695</v>
       </c>
     </row>
     <row r="328">
       <c r="A328" s="0" t="s">
-        <v>327</v>
+        <v>696</v>
       </c>
     </row>
     <row r="329">
       <c r="A329" s="0" t="s">
-        <v>328</v>
+        <v>697</v>
       </c>
     </row>
     <row r="330">
       <c r="A330" s="0" t="s">
-        <v>329</v>
+        <v>698</v>
       </c>
     </row>
     <row r="331">
       <c r="A331" s="0" t="s">
-        <v>330</v>
+        <v>699</v>
       </c>
     </row>
     <row r="332">
       <c r="A332" s="0" t="s">
-        <v>331</v>
+        <v>700</v>
       </c>
     </row>
     <row r="333">
       <c r="A333" s="0" t="s">
-        <v>332</v>
+        <v>701</v>
       </c>
     </row>
     <row r="334">
       <c r="A334" s="0" t="s">
-        <v>333</v>
+        <v>702</v>
       </c>
     </row>
     <row r="335">
       <c r="A335" s="0" t="s">
-        <v>334</v>
+        <v>703</v>
       </c>
     </row>
     <row r="336">
       <c r="A336" s="0" t="s">
-        <v>335</v>
+        <v>704</v>
       </c>
     </row>
     <row r="337">
       <c r="A337" s="0" t="s">
-        <v>336</v>
+        <v>705</v>
       </c>
     </row>
     <row r="338">
       <c r="A338" s="0" t="s">
-        <v>337</v>
+        <v>706</v>
       </c>
     </row>
     <row r="339">
       <c r="A339" s="0" t="s">
-        <v>338</v>
+        <v>707</v>
       </c>
     </row>
     <row r="340">
       <c r="A340" s="0" t="s">
-        <v>339</v>
+        <v>708</v>
       </c>
     </row>
     <row r="341">
       <c r="A341" s="0" t="s">
-        <v>340</v>
+        <v>709</v>
       </c>
     </row>
     <row r="342">
       <c r="A342" s="0" t="s">
-        <v>341</v>
+        <v>710</v>
       </c>
     </row>
     <row r="343">
       <c r="A343" s="0" t="s">
-        <v>342</v>
+        <v>711</v>
       </c>
     </row>
     <row r="344">
       <c r="A344" s="0" t="s">
-        <v>343</v>
+        <v>712</v>
       </c>
     </row>
     <row r="345">
       <c r="A345" s="0" t="s">
-        <v>344</v>
+        <v>713</v>
       </c>
     </row>
     <row r="346">
       <c r="A346" s="0" t="s">
-        <v>345</v>
+        <v>714</v>
       </c>
     </row>
     <row r="347">
       <c r="A347" s="0" t="s">
-        <v>346</v>
+        <v>715</v>
       </c>
     </row>
     <row r="348">
       <c r="A348" s="0" t="s">
-        <v>347</v>
+        <v>716</v>
       </c>
     </row>
     <row r="349">
       <c r="A349" s="0" t="s">
-        <v>348</v>
+        <v>717</v>
       </c>
     </row>
     <row r="350">
       <c r="A350" s="0" t="s">
-        <v>349</v>
+        <v>718</v>
       </c>
     </row>
     <row r="351">
       <c r="A351" s="0" t="s">
-        <v>350</v>
+        <v>719</v>
       </c>
     </row>
     <row r="352">
       <c r="A352" s="0" t="s">
-        <v>351</v>
+        <v>720</v>
       </c>
     </row>
     <row r="353">
       <c r="A353" s="0" t="s">
-        <v>352</v>
+        <v>721</v>
       </c>
     </row>
     <row r="354">
       <c r="A354" s="0" t="s">
-        <v>353</v>
+        <v>722</v>
       </c>
     </row>
     <row r="355">
       <c r="A355" s="0" t="s">
-        <v>354</v>
+        <v>723</v>
       </c>
     </row>
     <row r="356">
       <c r="A356" s="0" t="s">
-        <v>355</v>
+        <v>724</v>
       </c>
     </row>
     <row r="357">
       <c r="A357" s="0" t="s">
-        <v>356</v>
+        <v>725</v>
       </c>
     </row>
     <row r="358">
       <c r="A358" s="0" t="s">
-        <v>357</v>
+        <v>726</v>
       </c>
     </row>
     <row r="359">
       <c r="A359" s="0" t="s">
-        <v>358</v>
+        <v>727</v>
       </c>
     </row>
     <row r="360">
       <c r="A360" s="0" t="s">
-        <v>359</v>
+        <v>728</v>
       </c>
     </row>
     <row r="361">
       <c r="A361" s="0" t="s">
-        <v>360</v>
+        <v>729</v>
       </c>
     </row>
     <row r="362">
       <c r="A362" s="0" t="s">
-        <v>361</v>
+        <v>730</v>
       </c>
     </row>
     <row r="363">
       <c r="A363" s="0" t="s">
-        <v>362</v>
+        <v>731</v>
       </c>
     </row>
     <row r="364">
       <c r="A364" s="0" t="s">
-        <v>363</v>
+        <v>732</v>
       </c>
     </row>
     <row r="365">
       <c r="A365" s="0" t="s">
-        <v>364</v>
+        <v>733</v>
       </c>
     </row>
     <row r="366">
       <c r="A366" s="0" t="s">
-        <v>365</v>
+        <v>734</v>
       </c>
     </row>
     <row r="367">
       <c r="A367" s="0" t="s">
-        <v>366</v>
+        <v>735</v>
       </c>
     </row>
     <row r="368">
       <c r="A368" s="0" t="s">
-        <v>367</v>
+        <v>736</v>
       </c>
     </row>
     <row r="369">
       <c r="A369" s="0" t="s">
-        <v>368</v>
+        <v>737</v>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" s="0" t="s">
+        <v>738</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test with Alicia's code
</commit_message>
<xml_diff>
--- a/Data/ENS_ID_HKG.xlsx
+++ b/Data/ENS_ID_HKG.xlsx
@@ -13,7 +13,1117 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="739">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1109" uniqueCount="1109">
+  <si>
+    <t>ENSG00000149313</t>
+  </si>
+  <si>
+    <t>ENSG00000100997</t>
+  </si>
+  <si>
+    <t>ENSG00000177646</t>
+  </si>
+  <si>
+    <t>ENSG00000161533</t>
+  </si>
+  <si>
+    <t>ENSG00000197894</t>
+  </si>
+  <si>
+    <t>ENSG00000182551</t>
+  </si>
+  <si>
+    <t>ENSG00000181915</t>
+  </si>
+  <si>
+    <t>ENSG00000204310</t>
+  </si>
+  <si>
+    <t>ENSG00000160216</t>
+  </si>
+  <si>
+    <t>ENSG00000101444</t>
+  </si>
+  <si>
+    <t>ENSG00000004455</t>
+  </si>
+  <si>
+    <t>ENSG00000147853</t>
+  </si>
+  <si>
+    <t>ENSG00000117448</t>
+  </si>
+  <si>
+    <t>ENSG00000053371</t>
+  </si>
+  <si>
+    <t>ENSG00000143149</t>
+  </si>
+  <si>
+    <t>ENSG00000149925</t>
+  </si>
+  <si>
+    <t>ENSG00000159461</t>
+  </si>
+  <si>
+    <t>ENSG00000141552</t>
+  </si>
+  <si>
+    <t>ENSG00000166747</t>
+  </si>
+  <si>
+    <t>ENSG00000198931</t>
+  </si>
+  <si>
+    <t>ENSG00000095139</t>
+  </si>
+  <si>
+    <t>ENSG00000116539</t>
+  </si>
+  <si>
+    <t>ENSG00000107669</t>
+  </si>
+  <si>
+    <t>ENSG00000099624</t>
+  </si>
+  <si>
+    <t>ENSG00000124172</t>
+  </si>
+  <si>
+    <t>ENSG00000159199</t>
+  </si>
+  <si>
+    <t>ENSG00000169020</t>
+  </si>
+  <si>
+    <t>ENSG00000241468</t>
+  </si>
+  <si>
+    <t>ENSG00000167283</t>
+  </si>
+  <si>
+    <t>ENSG00000167863</t>
+  </si>
+  <si>
+    <t>ENSG00000154723</t>
+  </si>
+  <si>
+    <t>ENSG00000241837</t>
+  </si>
+  <si>
+    <t>ENSG00000071553</t>
+  </si>
+  <si>
+    <t>ENSG00000117410</t>
+  </si>
+  <si>
+    <t>ENSG00000185883</t>
+  </si>
+  <si>
+    <t>ENSG00000159720</t>
+  </si>
+  <si>
+    <t>ENSG00000113732</t>
+  </si>
+  <si>
+    <t>ENSG00000147416</t>
+  </si>
+  <si>
+    <t>ENSG00000131100</t>
+  </si>
+  <si>
+    <t>ENSG00000128524</t>
+  </si>
+  <si>
+    <t>ENSG00000136888</t>
+  </si>
+  <si>
+    <t>ENSG00000158850</t>
+  </si>
+  <si>
+    <t>ENSG00000158470</t>
+  </si>
+  <si>
+    <t>ENSG00000027847</t>
+  </si>
+  <si>
+    <t>ENSG00000174684</t>
+  </si>
+  <si>
+    <t>ENSG00000185825</t>
+  </si>
+  <si>
+    <t>ENSG00000103507</t>
+  </si>
+  <si>
+    <t>ENSG00000164039</t>
+  </si>
+  <si>
+    <t>ENSG00000172331</t>
+  </si>
+  <si>
+    <t>ENSG00000198668</t>
+  </si>
+  <si>
+    <t>ENSG00000160014</t>
+  </si>
+  <si>
+    <t>ENSG00000145439</t>
+  </si>
+  <si>
+    <t>ENSG00000099804</t>
+  </si>
+  <si>
+    <t>ENSG00000103502</t>
+  </si>
+  <si>
+    <t>ENSG00000101290</t>
+  </si>
+  <si>
+    <t>ENSG00000100422</t>
+  </si>
+  <si>
+    <t>ENSG00000143418</t>
+  </si>
+  <si>
+    <t>ENSG00000111726</t>
+  </si>
+  <si>
+    <t>ENSG00000162368</t>
+  </si>
+  <si>
+    <t>ENSG00000137200</t>
+  </si>
+  <si>
+    <t>ENSG00000173786</t>
+  </si>
+  <si>
+    <t>ENSG00000068120</t>
+  </si>
+  <si>
+    <t>ENSG00000093010</t>
+  </si>
+  <si>
+    <t>ENSG00000184432</t>
+  </si>
+  <si>
+    <t>ENSG00000105669</t>
+  </si>
+  <si>
+    <t>ENSG00000181789</t>
+  </si>
+  <si>
+    <t>ENSG00000110871</t>
+  </si>
+  <si>
+    <t>ENSG00000131143</t>
+  </si>
+  <si>
+    <t>ENSG00000178741</t>
+  </si>
+  <si>
+    <t>ENSG00000135940</t>
+  </si>
+  <si>
+    <t>ENSG00000111775</t>
+  </si>
+  <si>
+    <t>ENSG00000126267</t>
+  </si>
+  <si>
+    <t>ENSG00000131174</t>
+  </si>
+  <si>
+    <t>ENSG00000127184</t>
+  </si>
+  <si>
+    <t>ENSG00000176340</t>
+  </si>
+  <si>
+    <t>ENSG00000005339</t>
+  </si>
+  <si>
+    <t>ENSG00000169826</t>
+  </si>
+  <si>
+    <t>ENSG00000133275</t>
+  </si>
+  <si>
+    <t>ENSG00000159692</t>
+  </si>
+  <si>
+    <t>ENSG00000164733</t>
+  </si>
+  <si>
+    <t>ENSG00000117984</t>
+  </si>
+  <si>
+    <t>ENSG00000101160</t>
+  </si>
+  <si>
+    <t>ENSG00000159348</t>
+  </si>
+  <si>
+    <t>ENSG00000100243</t>
+  </si>
+  <si>
+    <t>ENSG00000179091</t>
+  </si>
+  <si>
+    <t>ENSG00000129562</t>
+  </si>
+  <si>
+    <t>ENSG00000129187</t>
+  </si>
+  <si>
+    <t>ENSG00000179958</t>
+  </si>
+  <si>
+    <t>ENSG00000143753</t>
+  </si>
+  <si>
+    <t>ENSG00000095059</t>
+  </si>
+  <si>
+    <t>ENSG00000091140</t>
+  </si>
+  <si>
+    <t>ENSG00000119689</t>
+  </si>
+  <si>
+    <t>ENSG00000000419</t>
+  </si>
+  <si>
+    <t>ENSG00000179085</t>
+  </si>
+  <si>
+    <t>ENSG00000144048</t>
+  </si>
+  <si>
+    <t>ENSG00000128951</t>
+  </si>
+  <si>
+    <t>ENSG00000104823</t>
+  </si>
+  <si>
+    <t>ENSG00000156508</t>
+  </si>
+  <si>
+    <t>ENSG00000167658</t>
+  </si>
+  <si>
+    <t>ENSG00000243056</t>
+  </si>
+  <si>
+    <t>ENSG00000066322</t>
+  </si>
+  <si>
+    <t>ENSG00000074800</t>
+  </si>
+  <si>
+    <t>ENSG00000197217</t>
+  </si>
+  <si>
+    <t>ENSG00000139684</t>
+  </si>
+  <si>
+    <t>ENSG00000105379</t>
+  </si>
+  <si>
+    <t>ENSG00000116199</t>
+  </si>
+  <si>
+    <t>ENSG00000179115</t>
+  </si>
+  <si>
+    <t>ENSG00000088832</t>
+  </si>
+  <si>
+    <t>ENSG00000105701</t>
+  </si>
+  <si>
+    <t>ENSG00000141560</t>
+  </si>
+  <si>
+    <t>ENSG00000141349</t>
+  </si>
+  <si>
+    <t>ENSG00000171298</t>
+  </si>
+  <si>
+    <t>ENSG00000141429</t>
+  </si>
+  <si>
+    <t>ENSG00000178234</t>
+  </si>
+  <si>
+    <t>ENSG00000111640</t>
+  </si>
+  <si>
+    <t>ENSG00000070610</t>
+  </si>
+  <si>
+    <t>ENSG00000006007</t>
+  </si>
+  <si>
+    <t>ENSG00000119392</t>
+  </si>
+  <si>
+    <t>ENSG00000124767</t>
+  </si>
+  <si>
+    <t>ENSG00000023572</t>
+  </si>
+  <si>
+    <t>ENSG00000116906</t>
+  </si>
+  <si>
+    <t>ENSG00000197858</t>
+  </si>
+  <si>
+    <t>ENSG00000158669</t>
+  </si>
+  <si>
+    <t>ENSG00000105220</t>
+  </si>
+  <si>
+    <t>ENSG00000233276</t>
+  </si>
+  <si>
+    <t>ENSG00000167468</t>
+  </si>
+  <si>
+    <t>ENSG00000137106</t>
+  </si>
+  <si>
+    <t>ENSG00000173020</t>
+  </si>
+  <si>
+    <t>ENSG00000100983</t>
+  </si>
+  <si>
+    <t>ENSG00000197448</t>
+  </si>
+  <si>
+    <t>ENSG00000148834</t>
+  </si>
+  <si>
+    <t>ENSG00000143774</t>
+  </si>
+  <si>
+    <t>ENSG00000084754</t>
+  </si>
+  <si>
+    <t>ENSG00000063854</t>
+  </si>
+  <si>
+    <t>ENSG00000128708</t>
+  </si>
+  <si>
+    <t>ENSG00000115677</t>
+  </si>
+  <si>
+    <t>ENSG00000092148</t>
+  </si>
+  <si>
+    <t>ENSG00000146066</t>
+  </si>
+  <si>
+    <t>ENSG00000149084</t>
+  </si>
+  <si>
+    <t>ENSG00000086758</t>
+  </si>
+  <si>
+    <t>ENSG00000116237</t>
+  </si>
+  <si>
+    <t>ENSG00000101365</t>
+  </si>
+  <si>
+    <t>ENSG00000067829</t>
+  </si>
+  <si>
+    <t>ENSG00000010404</t>
+  </si>
+  <si>
+    <t>ENSG00000132376</t>
+  </si>
+  <si>
+    <t>ENSG00000068745</t>
+  </si>
+  <si>
+    <t>ENSG00000078747</t>
+  </si>
+  <si>
+    <t>ENSG00000100605</t>
+  </si>
+  <si>
+    <t>ENSG00000103510</t>
+  </si>
+  <si>
+    <t>ENSG00000025800</t>
+  </si>
+  <si>
+    <t>ENSG00000123684</t>
+  </si>
+  <si>
+    <t>ENSG00000198162</t>
+  </si>
+  <si>
+    <t>ENSG00000131844</t>
+  </si>
+  <si>
+    <t>ENSG00000146701</t>
+  </si>
+  <si>
+    <t>ENSG00000102858</t>
+  </si>
+  <si>
+    <t>ENSG00000143198</t>
+  </si>
+  <si>
+    <t>ENSG00000240972</t>
+  </si>
+  <si>
+    <t>ENSG00000133606</t>
+  </si>
+  <si>
+    <t>ENSG00000075975</t>
+  </si>
+  <si>
+    <t>ENSG00000143158</t>
+  </si>
+  <si>
+    <t>ENSG00000167862</t>
+  </si>
+  <si>
+    <t>ENSG00000039123</t>
+  </si>
+  <si>
+    <t>ENSG00000090432</t>
+  </si>
+  <si>
+    <t>ENSG00000005810</t>
+  </si>
+  <si>
+    <t>ENSG00000135372</t>
+  </si>
+  <si>
+    <t>ENSG00000070614</t>
+  </si>
+  <si>
+    <t>ENSG00000125356</t>
+  </si>
+  <si>
+    <t>ENSG00000174886</t>
+  </si>
+  <si>
+    <t>ENSG00000184752</t>
+  </si>
+  <si>
+    <t>ENSG00000131495</t>
+  </si>
+  <si>
+    <t>ENSG00000189043</t>
+  </si>
+  <si>
+    <t>ENSG00000128609</t>
+  </si>
+  <si>
+    <t>ENSG00000119421</t>
+  </si>
+  <si>
+    <t>ENSG00000004779</t>
+  </si>
+  <si>
+    <t>ENSG00000183648</t>
+  </si>
+  <si>
+    <t>ENSG00000140990</t>
+  </si>
+  <si>
+    <t>ENSG00000147123</t>
+  </si>
+  <si>
+    <t>ENSG00000090266</t>
+  </si>
+  <si>
+    <t>ENSG00000119013</t>
+  </si>
+  <si>
+    <t>ENSG00000065518</t>
+  </si>
+  <si>
+    <t>ENSG00000165264</t>
+  </si>
+  <si>
+    <t>ENSG00000099795</t>
+  </si>
+  <si>
+    <t>ENSG00000166136</t>
+  </si>
+  <si>
+    <t>ENSG00000147684</t>
+  </si>
+  <si>
+    <t>ENSG00000151366</t>
+  </si>
+  <si>
+    <t>ENSG00000213619</t>
+  </si>
+  <si>
+    <t>ENSG00000145494</t>
+  </si>
+  <si>
+    <t>ENSG00000110717</t>
+  </si>
+  <si>
+    <t>ENSG00000160194</t>
+  </si>
+  <si>
+    <t>ENSG00000204386</t>
+  </si>
+  <si>
+    <t>ENSG00000243678</t>
+  </si>
+  <si>
+    <t>ENSG00000136448</t>
+  </si>
+  <si>
+    <t>ENSG00000141279</t>
+  </si>
+  <si>
+    <t>ENSG00000076685</t>
+  </si>
+  <si>
+    <t>ENSG00000170502</t>
+  </si>
+  <si>
+    <t>ENSG00000069248</t>
+  </si>
+  <si>
+    <t>ENSG00000124789</t>
+  </si>
+  <si>
+    <t>ENSG00000139496</t>
+  </si>
+  <si>
+    <t>ENSG00000198408</t>
+  </si>
+  <si>
+    <t>ENSG00000105953</t>
+  </si>
+  <si>
+    <t>ENSG00000147162</t>
+  </si>
+  <si>
+    <t>ENSG00000068308</t>
+  </si>
+  <si>
+    <t>ENSG00000185624</t>
+  </si>
+  <si>
+    <t>ENSG00000007168</t>
+  </si>
+  <si>
+    <t>ENSG00000168092</t>
+  </si>
+  <si>
+    <t>ENSG00000120137</t>
+  </si>
+  <si>
+    <t>ENSG00000090060</t>
+  </si>
+  <si>
+    <t>ENSG00000143799</t>
+  </si>
+  <si>
+    <t>ENSG00000166228</t>
+  </si>
+  <si>
+    <t>ENSG00000120265</t>
+  </si>
+  <si>
+    <t>ENSG00000116005</t>
+  </si>
+  <si>
+    <t>ENSG00000161217</t>
+  </si>
+  <si>
+    <t>ENSG00000131828</t>
+  </si>
+  <si>
+    <t>ENSG00000167004</t>
+  </si>
+  <si>
+    <t>ENSG00000143870</t>
+  </si>
+  <si>
+    <t>ENSG00000141959</t>
+  </si>
+  <si>
+    <t>ENSG00000171314</t>
+  </si>
+  <si>
+    <t>ENSG00000130313</t>
+  </si>
+  <si>
+    <t>ENSG00000155252</t>
+  </si>
+  <si>
+    <t>ENSG00000100564</t>
+  </si>
+  <si>
+    <t>ENSG00000127445</t>
+  </si>
+  <si>
+    <t>ENSG00000102309</t>
+  </si>
+  <si>
+    <t>ENSG00000165782</t>
+  </si>
+  <si>
+    <t>ENSG00000186111</t>
+  </si>
+  <si>
+    <t>ENSG00000103066</t>
+  </si>
+  <si>
+    <t>ENSG00000124181</t>
+  </si>
+  <si>
+    <t>ENSG00000083444</t>
+  </si>
+  <si>
+    <t>ENSG00000106397</t>
+  </si>
+  <si>
+    <t>ENSG00000100417</t>
+  </si>
+  <si>
+    <t>ENSG00000165688</t>
+  </si>
+  <si>
+    <t>ENSG00000163344</t>
+  </si>
+  <si>
+    <t>ENSG00000106628</t>
+  </si>
+  <si>
+    <t>ENSG00000148229</t>
+  </si>
+  <si>
+    <t>ENSG00000186184</t>
+  </si>
+  <si>
+    <t>ENSG00000137054</t>
+  </si>
+  <si>
+    <t>ENSG00000102978</t>
+  </si>
+  <si>
+    <t>ENSG00000100142</t>
+  </si>
+  <si>
+    <t>ENSG00000105258</t>
+  </si>
+  <si>
+    <t>ENSG00000005075</t>
+  </si>
+  <si>
+    <t>ENSG00000147669</t>
+  </si>
+  <si>
+    <t>ENSG00000177700</t>
+  </si>
+  <si>
+    <t>ENSG00000186141</t>
+  </si>
+  <si>
+    <t>ENSG00000121851</t>
+  </si>
+  <si>
+    <t>ENSG00000085998</t>
+  </si>
+  <si>
+    <t>ENSG00000180817</t>
+  </si>
+  <si>
+    <t>ENSG00000196262</t>
+  </si>
+  <si>
+    <t>ENSG00000166794</t>
+  </si>
+  <si>
+    <t>ENSG00000171497</t>
+  </si>
+  <si>
+    <t>ENSG00000171960</t>
+  </si>
+  <si>
+    <t>ENSG00000131013</t>
+  </si>
+  <si>
+    <t>ENSG00000131238</t>
+  </si>
+  <si>
+    <t>ENSG00000117450</t>
+  </si>
+  <si>
+    <t>ENSG00000167815</t>
+  </si>
+  <si>
+    <t>ENSG00000126432</t>
+  </si>
+  <si>
+    <t>ENSG00000117592</t>
+  </si>
+  <si>
+    <t>ENSG00000085377</t>
+  </si>
+  <si>
+    <t>ENSG00000147224</t>
+  </si>
+  <si>
+    <t>ENSG00000197746</t>
+  </si>
+  <si>
+    <t>ENSG00000174915</t>
+  </si>
+  <si>
+    <t>ENSG00000171862</t>
+  </si>
+  <si>
+    <t>ENSG00000148334</t>
+  </si>
+  <si>
+    <t>ENSG00000110958</t>
+  </si>
+  <si>
+    <t>ENSG00000141378</t>
+  </si>
+  <si>
+    <t>ENSG00000143811</t>
+  </si>
+  <si>
+    <t>ENSG00000145337</t>
+  </si>
+  <si>
+    <t>ENSG00000017797</t>
+  </si>
+  <si>
+    <t>ENSG00000153201</t>
+  </si>
+  <si>
+    <t>ENSG00000240857</t>
+  </si>
+  <si>
+    <t>ENSG00000204227</t>
+  </si>
+  <si>
+    <t>ENSG00000070423</t>
+  </si>
+  <si>
+    <t>ENSG00000082996</t>
+  </si>
+  <si>
+    <t>ENSG00000170881</t>
+  </si>
+  <si>
+    <t>ENSG00000163162</t>
+  </si>
+  <si>
+    <t>ENSG00000108523</t>
+  </si>
+  <si>
+    <t>ENSG00000168159</t>
+  </si>
+  <si>
+    <t>ENSG00000034677</t>
+  </si>
+  <si>
+    <t>ENSG00000155827</t>
+  </si>
+  <si>
+    <t>ENSG00000011275</t>
+  </si>
+  <si>
+    <t>ENSG00000153574</t>
+  </si>
+  <si>
+    <t>ENSG00000241343</t>
+  </si>
+  <si>
+    <t>ENSG00000163902</t>
+  </si>
+  <si>
+    <t>ENSG00000118705</t>
+  </si>
+  <si>
+    <t>ENSG00000117118</t>
+  </si>
+  <si>
+    <t>ENSG00000204370</t>
+  </si>
+  <si>
+    <t>ENSG00000140612</t>
+  </si>
+  <si>
+    <t>ENSG00000157020</t>
+  </si>
+  <si>
+    <t>ENSG00000086475</t>
+  </si>
+  <si>
+    <t>ENSG00000099381</t>
+  </si>
+  <si>
+    <t>ENSG00000139718</t>
+  </si>
+  <si>
+    <t>ENSG00000168137</t>
+  </si>
+  <si>
+    <t>ENSG00000097033</t>
+  </si>
+  <si>
+    <t>ENSG00000181788</t>
+  </si>
+  <si>
+    <t>ENSG00000068903</t>
+  </si>
+  <si>
+    <t>ENSG00000108528</t>
+  </si>
+  <si>
+    <t>ENSG00000155287</t>
+  </si>
+  <si>
+    <t>ENSG00000075415</t>
+  </si>
+  <si>
+    <t>ENSG00000144659</t>
+  </si>
+  <si>
+    <t>ENSG00000005022</t>
+  </si>
+  <si>
+    <t>ENSG00000169100</t>
+  </si>
+  <si>
+    <t>ENSG00000164414</t>
+  </si>
+  <si>
+    <t>ENSG00000134294</t>
+  </si>
+  <si>
+    <t>ENSG00000143570</t>
+  </si>
+  <si>
+    <t>ENSG00000141424</t>
+  </si>
+  <si>
+    <t>ENSG00000112473</t>
+  </si>
+  <si>
+    <t>ENSG00000166311</t>
+  </si>
+  <si>
+    <t>ENSG00000198742</t>
+  </si>
+  <si>
+    <t>ENSG00000142168</t>
+  </si>
+  <si>
+    <t>ENSG00000118363</t>
+  </si>
+  <si>
+    <t>ENSG00000129128</t>
+  </si>
+  <si>
+    <t>ENSG00000116649</t>
+  </si>
+  <si>
+    <t>ENSG00000163527</t>
+  </si>
+  <si>
+    <t>ENSG00000103266</t>
+  </si>
+  <si>
+    <t>ENSG00000273841</t>
+  </si>
+  <si>
+    <t>ENSG00000177156</t>
+  </si>
+  <si>
+    <t>ENSG00000105254</t>
+  </si>
+  <si>
+    <t>ENSG00000112941</t>
+  </si>
+  <si>
+    <t>ENSG00000166479</t>
+  </si>
+  <si>
+    <t>ENSG00000173273</t>
+  </si>
+  <si>
+    <t>ENSG00000107854</t>
+  </si>
+  <si>
+    <t>ENSG00000111669</t>
+  </si>
+  <si>
+    <t>ENSG00000166340</t>
+  </si>
+  <si>
+    <t>ENSG00000047410</t>
+  </si>
+  <si>
+    <t>ENSG00000131653</t>
+  </si>
+  <si>
+    <t>ENSG00000153827</t>
+  </si>
+  <si>
+    <t>ENSG00000149016</t>
+  </si>
+  <si>
+    <t>ENSG00000100348</t>
+  </si>
+  <si>
+    <t>ENSG00000130985</t>
+  </si>
+  <si>
+    <t>ENSG00000126261</t>
+  </si>
+  <si>
+    <t>ENSG00000077721</t>
+  </si>
+  <si>
+    <t>ENSG00000119048</t>
+  </si>
+  <si>
+    <t>ENSG00000131508</t>
+  </si>
+  <si>
+    <t>ENSG00000109332</t>
+  </si>
+  <si>
+    <t>ENSG00000184182</t>
+  </si>
+  <si>
+    <t>ENSG00000132388</t>
+  </si>
+  <si>
+    <t>ENSG00000184787</t>
+  </si>
+  <si>
+    <t>ENSG00000186591</t>
+  </si>
+  <si>
+    <t>ENSG00000103275</t>
+  </si>
+  <si>
+    <t>ENSG00000198833</t>
+  </si>
+  <si>
+    <t>ENSG00000078140</t>
+  </si>
+  <si>
+    <t>ENSG00000185651</t>
+  </si>
+  <si>
+    <t>ENSG00000130725</t>
+  </si>
+  <si>
+    <t>ENSG00000175931</t>
+  </si>
+  <si>
+    <t>ENSG00000160714</t>
+  </si>
+  <si>
+    <t>ENSG00000107341</t>
+  </si>
+  <si>
+    <t>ENSG00000159202</t>
+  </si>
+  <si>
+    <t>ENSG00000009335</t>
+  </si>
+  <si>
+    <t>ENSG00000127481</t>
+  </si>
+  <si>
+    <t>ENSG00000169764</t>
+  </si>
+  <si>
+    <t>ENSG00000184076</t>
+  </si>
+  <si>
+    <t>ENSG00000127540</t>
+  </si>
+  <si>
+    <t>ENSG00000156467</t>
+  </si>
+  <si>
+    <t>ENSG00000173660</t>
+  </si>
+  <si>
+    <t>ENSG00000164405</t>
+  </si>
+  <si>
+    <t>ENSG00000126088</t>
+  </si>
+  <si>
+    <t>ENSG00000102226</t>
+  </si>
+  <si>
+    <t>ENSG00000152484</t>
+  </si>
+  <si>
+    <t>ENSG00000101557</t>
+  </si>
+  <si>
+    <t>ENSG00000124422</t>
+  </si>
+  <si>
+    <t>ENSG00000115464</t>
+  </si>
+  <si>
+    <t>ENSG00000114316</t>
+  </si>
+  <si>
+    <t>ENSG00000090686</t>
+  </si>
+  <si>
+    <t>ENSG00000187555</t>
+  </si>
+  <si>
+    <t>ENSG00000124486</t>
+  </si>
+  <si>
+    <t>ENSG00000167397</t>
+  </si>
+  <si>
+    <t>ENSG00000111237</t>
+  </si>
+  <si>
+    <t>ENSG00000106636</t>
+  </si>
+  <si>
+    <t>ENSG00000023041</t>
+  </si>
+  <si>
+    <t>ENSG00000153786</t>
+  </si>
+  <si>
+    <t>ENSG00000084073</t>
+  </si>
+  <si>
+    <t>ENSEMBL_ID</t>
+  </si>
   <si>
     <t>ENSG00000149313</t>
   </si>
@@ -2283,1852 +3393,1852 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>369</v>
+        <v>739</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>370</v>
+        <v>740</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>371</v>
+        <v>741</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>372</v>
+        <v>742</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>373</v>
+        <v>743</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>374</v>
+        <v>744</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>375</v>
+        <v>745</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>376</v>
+        <v>746</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>377</v>
+        <v>747</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>378</v>
+        <v>748</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>379</v>
+        <v>749</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>380</v>
+        <v>750</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>381</v>
+        <v>751</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>382</v>
+        <v>752</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>383</v>
+        <v>753</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>384</v>
+        <v>754</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="s">
-        <v>385</v>
+        <v>755</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="s">
-        <v>386</v>
+        <v>756</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="s">
-        <v>387</v>
+        <v>757</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="s">
-        <v>388</v>
+        <v>758</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="s">
-        <v>389</v>
+        <v>759</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="s">
-        <v>390</v>
+        <v>760</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="s">
-        <v>391</v>
+        <v>761</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="s">
-        <v>392</v>
+        <v>762</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="s">
-        <v>393</v>
+        <v>763</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="s">
-        <v>394</v>
+        <v>764</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="s">
-        <v>395</v>
+        <v>765</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="s">
-        <v>396</v>
+        <v>766</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0" t="s">
-        <v>397</v>
+        <v>767</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="s">
-        <v>398</v>
+        <v>768</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="s">
-        <v>399</v>
+        <v>769</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="s">
-        <v>400</v>
+        <v>770</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0" t="s">
-        <v>401</v>
+        <v>771</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0" t="s">
-        <v>402</v>
+        <v>772</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0" t="s">
-        <v>403</v>
+        <v>773</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0" t="s">
-        <v>404</v>
+        <v>774</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0" t="s">
-        <v>405</v>
+        <v>775</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0" t="s">
-        <v>406</v>
+        <v>776</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0" t="s">
-        <v>407</v>
+        <v>777</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0" t="s">
-        <v>408</v>
+        <v>778</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0" t="s">
-        <v>409</v>
+        <v>779</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0" t="s">
-        <v>410</v>
+        <v>780</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0" t="s">
-        <v>411</v>
+        <v>781</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0" t="s">
-        <v>412</v>
+        <v>782</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0" t="s">
-        <v>413</v>
+        <v>783</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0" t="s">
-        <v>414</v>
+        <v>784</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0" t="s">
-        <v>415</v>
+        <v>785</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0" t="s">
-        <v>416</v>
+        <v>786</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0" t="s">
-        <v>417</v>
+        <v>787</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0" t="s">
-        <v>418</v>
+        <v>788</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0" t="s">
-        <v>419</v>
+        <v>789</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0" t="s">
-        <v>420</v>
+        <v>790</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0" t="s">
-        <v>421</v>
+        <v>791</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0" t="s">
-        <v>422</v>
+        <v>792</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0" t="s">
-        <v>423</v>
+        <v>793</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0" t="s">
-        <v>424</v>
+        <v>794</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0" t="s">
-        <v>425</v>
+        <v>795</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0" t="s">
-        <v>426</v>
+        <v>796</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0" t="s">
-        <v>427</v>
+        <v>797</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0" t="s">
-        <v>428</v>
+        <v>798</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="0" t="s">
-        <v>429</v>
+        <v>799</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="0" t="s">
-        <v>430</v>
+        <v>800</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="0" t="s">
-        <v>431</v>
+        <v>801</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="0" t="s">
-        <v>432</v>
+        <v>802</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="0" t="s">
-        <v>433</v>
+        <v>803</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="0" t="s">
-        <v>434</v>
+        <v>804</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="0" t="s">
-        <v>435</v>
+        <v>805</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="0" t="s">
-        <v>436</v>
+        <v>806</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="0" t="s">
-        <v>437</v>
+        <v>807</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="0" t="s">
-        <v>438</v>
+        <v>808</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="0" t="s">
-        <v>439</v>
+        <v>809</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="0" t="s">
-        <v>440</v>
+        <v>810</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="0" t="s">
-        <v>441</v>
+        <v>811</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="0" t="s">
-        <v>442</v>
+        <v>812</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="0" t="s">
-        <v>443</v>
+        <v>813</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="0" t="s">
-        <v>444</v>
+        <v>814</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="0" t="s">
-        <v>445</v>
+        <v>815</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="0" t="s">
-        <v>446</v>
+        <v>816</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="0" t="s">
-        <v>447</v>
+        <v>817</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="0" t="s">
-        <v>448</v>
+        <v>818</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="0" t="s">
-        <v>449</v>
+        <v>819</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="0" t="s">
-        <v>450</v>
+        <v>820</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="0" t="s">
-        <v>451</v>
+        <v>821</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="0" t="s">
-        <v>452</v>
+        <v>822</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="0" t="s">
-        <v>453</v>
+        <v>823</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="0" t="s">
-        <v>454</v>
+        <v>824</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="0" t="s">
-        <v>455</v>
+        <v>825</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="0" t="s">
-        <v>456</v>
+        <v>826</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="0" t="s">
-        <v>457</v>
+        <v>827</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="0" t="s">
-        <v>458</v>
+        <v>828</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="0" t="s">
-        <v>459</v>
+        <v>829</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="0" t="s">
-        <v>460</v>
+        <v>830</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="0" t="s">
-        <v>461</v>
+        <v>831</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="0" t="s">
-        <v>462</v>
+        <v>832</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="0" t="s">
-        <v>463</v>
+        <v>833</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="0" t="s">
-        <v>464</v>
+        <v>834</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="0" t="s">
-        <v>465</v>
+        <v>835</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="0" t="s">
-        <v>466</v>
+        <v>836</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="0" t="s">
-        <v>467</v>
+        <v>837</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="0" t="s">
-        <v>468</v>
+        <v>838</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="0" t="s">
-        <v>469</v>
+        <v>839</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="0" t="s">
-        <v>470</v>
+        <v>840</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="0" t="s">
-        <v>471</v>
+        <v>841</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="0" t="s">
-        <v>472</v>
+        <v>842</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="0" t="s">
-        <v>473</v>
+        <v>843</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="0" t="s">
-        <v>474</v>
+        <v>844</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="0" t="s">
-        <v>475</v>
+        <v>845</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="0" t="s">
-        <v>476</v>
+        <v>846</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="0" t="s">
-        <v>477</v>
+        <v>847</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="0" t="s">
-        <v>478</v>
+        <v>848</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="0" t="s">
-        <v>479</v>
+        <v>849</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="0" t="s">
-        <v>480</v>
+        <v>850</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="0" t="s">
-        <v>481</v>
+        <v>851</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="0" t="s">
-        <v>482</v>
+        <v>852</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="0" t="s">
-        <v>483</v>
+        <v>853</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="0" t="s">
-        <v>484</v>
+        <v>854</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="0" t="s">
-        <v>485</v>
+        <v>855</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="0" t="s">
-        <v>486</v>
+        <v>856</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="0" t="s">
-        <v>487</v>
+        <v>857</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="0" t="s">
-        <v>488</v>
+        <v>858</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="0" t="s">
-        <v>489</v>
+        <v>859</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="0" t="s">
-        <v>490</v>
+        <v>860</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="0" t="s">
-        <v>491</v>
+        <v>861</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="0" t="s">
-        <v>492</v>
+        <v>862</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="0" t="s">
-        <v>493</v>
+        <v>863</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="0" t="s">
-        <v>494</v>
+        <v>864</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="0" t="s">
-        <v>495</v>
+        <v>865</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="0" t="s">
-        <v>496</v>
+        <v>866</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="0" t="s">
-        <v>497</v>
+        <v>867</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="0" t="s">
-        <v>498</v>
+        <v>868</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="0" t="s">
-        <v>499</v>
+        <v>869</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="0" t="s">
-        <v>500</v>
+        <v>870</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="0" t="s">
-        <v>501</v>
+        <v>871</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="0" t="s">
-        <v>502</v>
+        <v>872</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="0" t="s">
-        <v>503</v>
+        <v>873</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="0" t="s">
-        <v>504</v>
+        <v>874</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="0" t="s">
-        <v>505</v>
+        <v>875</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="0" t="s">
-        <v>506</v>
+        <v>876</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="0" t="s">
-        <v>507</v>
+        <v>877</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="0" t="s">
-        <v>508</v>
+        <v>878</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="0" t="s">
-        <v>509</v>
+        <v>879</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="0" t="s">
-        <v>510</v>
+        <v>880</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="0" t="s">
-        <v>511</v>
+        <v>881</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="0" t="s">
-        <v>512</v>
+        <v>882</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="0" t="s">
-        <v>513</v>
+        <v>883</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="0" t="s">
-        <v>514</v>
+        <v>884</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="0" t="s">
-        <v>515</v>
+        <v>885</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="0" t="s">
-        <v>516</v>
+        <v>886</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="0" t="s">
-        <v>517</v>
+        <v>887</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="0" t="s">
-        <v>518</v>
+        <v>888</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="0" t="s">
-        <v>519</v>
+        <v>889</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="0" t="s">
-        <v>520</v>
+        <v>890</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="0" t="s">
-        <v>521</v>
+        <v>891</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="0" t="s">
-        <v>522</v>
+        <v>892</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="0" t="s">
-        <v>523</v>
+        <v>893</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="0" t="s">
-        <v>524</v>
+        <v>894</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="0" t="s">
-        <v>525</v>
+        <v>895</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="0" t="s">
-        <v>526</v>
+        <v>896</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="0" t="s">
-        <v>527</v>
+        <v>897</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="0" t="s">
-        <v>528</v>
+        <v>898</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="0" t="s">
-        <v>529</v>
+        <v>899</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="0" t="s">
-        <v>530</v>
+        <v>900</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="0" t="s">
-        <v>531</v>
+        <v>901</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="0" t="s">
-        <v>532</v>
+        <v>902</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="0" t="s">
-        <v>533</v>
+        <v>903</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="0" t="s">
-        <v>534</v>
+        <v>904</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="0" t="s">
-        <v>535</v>
+        <v>905</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="0" t="s">
-        <v>536</v>
+        <v>906</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="0" t="s">
-        <v>537</v>
+        <v>907</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="0" t="s">
-        <v>538</v>
+        <v>908</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="0" t="s">
-        <v>539</v>
+        <v>909</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="0" t="s">
-        <v>540</v>
+        <v>910</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="0" t="s">
-        <v>541</v>
+        <v>911</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="0" t="s">
-        <v>542</v>
+        <v>912</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="0" t="s">
-        <v>543</v>
+        <v>913</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="0" t="s">
-        <v>544</v>
+        <v>914</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="0" t="s">
-        <v>545</v>
+        <v>915</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="0" t="s">
-        <v>546</v>
+        <v>916</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="0" t="s">
-        <v>547</v>
+        <v>917</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="0" t="s">
-        <v>548</v>
+        <v>918</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="0" t="s">
-        <v>549</v>
+        <v>919</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="0" t="s">
-        <v>550</v>
+        <v>920</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="0" t="s">
-        <v>551</v>
+        <v>921</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="0" t="s">
-        <v>552</v>
+        <v>922</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="0" t="s">
-        <v>553</v>
+        <v>923</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="0" t="s">
-        <v>554</v>
+        <v>924</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="0" t="s">
-        <v>555</v>
+        <v>925</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="0" t="s">
-        <v>556</v>
+        <v>926</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="0" t="s">
-        <v>557</v>
+        <v>927</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="0" t="s">
-        <v>558</v>
+        <v>928</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="0" t="s">
-        <v>559</v>
+        <v>929</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="0" t="s">
-        <v>560</v>
+        <v>930</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="0" t="s">
-        <v>561</v>
+        <v>931</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="0" t="s">
-        <v>562</v>
+        <v>932</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="0" t="s">
-        <v>563</v>
+        <v>933</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="0" t="s">
-        <v>564</v>
+        <v>934</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="0" t="s">
-        <v>565</v>
+        <v>935</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="0" t="s">
-        <v>566</v>
+        <v>936</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="0" t="s">
-        <v>567</v>
+        <v>937</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="0" t="s">
-        <v>568</v>
+        <v>938</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="0" t="s">
-        <v>569</v>
+        <v>939</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="0" t="s">
-        <v>570</v>
+        <v>940</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="0" t="s">
-        <v>571</v>
+        <v>941</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="0" t="s">
-        <v>572</v>
+        <v>942</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="0" t="s">
-        <v>573</v>
+        <v>943</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="0" t="s">
-        <v>574</v>
+        <v>944</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="0" t="s">
-        <v>575</v>
+        <v>945</v>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="0" t="s">
-        <v>576</v>
+        <v>946</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="0" t="s">
-        <v>577</v>
+        <v>947</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="0" t="s">
-        <v>578</v>
+        <v>948</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="0" t="s">
-        <v>579</v>
+        <v>949</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="0" t="s">
-        <v>580</v>
+        <v>950</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="0" t="s">
-        <v>581</v>
+        <v>951</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="0" t="s">
-        <v>582</v>
+        <v>952</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="0" t="s">
-        <v>583</v>
+        <v>953</v>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="0" t="s">
-        <v>584</v>
+        <v>954</v>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="0" t="s">
-        <v>585</v>
+        <v>955</v>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="0" t="s">
-        <v>586</v>
+        <v>956</v>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="0" t="s">
-        <v>587</v>
+        <v>957</v>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="0" t="s">
-        <v>588</v>
+        <v>958</v>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="0" t="s">
-        <v>589</v>
+        <v>959</v>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="0" t="s">
-        <v>590</v>
+        <v>960</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="0" t="s">
-        <v>591</v>
+        <v>961</v>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="0" t="s">
-        <v>592</v>
+        <v>962</v>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="0" t="s">
-        <v>593</v>
+        <v>963</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="0" t="s">
-        <v>594</v>
+        <v>964</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="0" t="s">
-        <v>595</v>
+        <v>965</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="0" t="s">
-        <v>596</v>
+        <v>966</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="0" t="s">
-        <v>597</v>
+        <v>967</v>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="0" t="s">
-        <v>598</v>
+        <v>968</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="0" t="s">
-        <v>599</v>
+        <v>969</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="0" t="s">
-        <v>600</v>
+        <v>970</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="0" t="s">
-        <v>601</v>
+        <v>971</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="0" t="s">
-        <v>602</v>
+        <v>972</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="0" t="s">
-        <v>603</v>
+        <v>973</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="0" t="s">
-        <v>604</v>
+        <v>974</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="0" t="s">
-        <v>605</v>
+        <v>975</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="0" t="s">
-        <v>606</v>
+        <v>976</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="0" t="s">
-        <v>607</v>
+        <v>977</v>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="0" t="s">
-        <v>608</v>
+        <v>978</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="0" t="s">
-        <v>609</v>
+        <v>979</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="0" t="s">
-        <v>610</v>
+        <v>980</v>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="0" t="s">
-        <v>611</v>
+        <v>981</v>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="0" t="s">
-        <v>612</v>
+        <v>982</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="0" t="s">
-        <v>613</v>
+        <v>983</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="0" t="s">
-        <v>614</v>
+        <v>984</v>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="0" t="s">
-        <v>615</v>
+        <v>985</v>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="0" t="s">
-        <v>616</v>
+        <v>986</v>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="0" t="s">
-        <v>617</v>
+        <v>987</v>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="0" t="s">
-        <v>618</v>
+        <v>988</v>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="0" t="s">
-        <v>619</v>
+        <v>989</v>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="0" t="s">
-        <v>620</v>
+        <v>990</v>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="0" t="s">
-        <v>621</v>
+        <v>991</v>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="0" t="s">
-        <v>622</v>
+        <v>992</v>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="0" t="s">
-        <v>623</v>
+        <v>993</v>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="0" t="s">
-        <v>624</v>
+        <v>994</v>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="0" t="s">
-        <v>625</v>
+        <v>995</v>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="0" t="s">
-        <v>626</v>
+        <v>996</v>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="0" t="s">
-        <v>627</v>
+        <v>997</v>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="0" t="s">
-        <v>628</v>
+        <v>998</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="0" t="s">
-        <v>629</v>
+        <v>999</v>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="0" t="s">
-        <v>630</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="0" t="s">
-        <v>631</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="0" t="s">
-        <v>632</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="0" t="s">
-        <v>633</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="0" t="s">
-        <v>634</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="0" t="s">
-        <v>635</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="0" t="s">
-        <v>636</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="0" t="s">
-        <v>637</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="0" t="s">
-        <v>638</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="0" t="s">
-        <v>639</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="0" t="s">
-        <v>640</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="0" t="s">
-        <v>641</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="0" t="s">
-        <v>642</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="0" t="s">
-        <v>643</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="0" t="s">
-        <v>644</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="0" t="s">
-        <v>645</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="0" t="s">
-        <v>646</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="0" t="s">
-        <v>647</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="0" t="s">
-        <v>648</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="0" t="s">
-        <v>649</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="0" t="s">
-        <v>650</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="0" t="s">
-        <v>651</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="0" t="s">
-        <v>652</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="0" t="s">
-        <v>653</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="0" t="s">
-        <v>654</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="0" t="s">
-        <v>655</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="0" t="s">
-        <v>656</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="0" t="s">
-        <v>657</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="0" t="s">
-        <v>658</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="0" t="s">
-        <v>659</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="0" t="s">
-        <v>660</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="0" t="s">
-        <v>661</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="0" t="s">
-        <v>662</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="0" t="s">
-        <v>663</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="0" t="s">
-        <v>664</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="0" t="s">
-        <v>665</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="0" t="s">
-        <v>666</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="0" t="s">
-        <v>667</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="0" t="s">
-        <v>668</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="0" t="s">
-        <v>669</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="0" t="s">
-        <v>670</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="0" t="s">
-        <v>671</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="0" t="s">
-        <v>672</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="0" t="s">
-        <v>673</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="0" t="s">
-        <v>674</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="0" t="s">
-        <v>675</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="0" t="s">
-        <v>676</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="0" t="s">
-        <v>677</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="0" t="s">
-        <v>678</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="0" t="s">
-        <v>679</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="0" t="s">
-        <v>680</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="0" t="s">
-        <v>681</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="0" t="s">
-        <v>682</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="0" t="s">
-        <v>683</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="316">
       <c r="A316" s="0" t="s">
-        <v>684</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="317">
       <c r="A317" s="0" t="s">
-        <v>685</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="318">
       <c r="A318" s="0" t="s">
-        <v>686</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="319">
       <c r="A319" s="0" t="s">
-        <v>687</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="320">
       <c r="A320" s="0" t="s">
-        <v>688</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="321">
       <c r="A321" s="0" t="s">
-        <v>689</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="322">
       <c r="A322" s="0" t="s">
-        <v>690</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="323">
       <c r="A323" s="0" t="s">
-        <v>691</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="324">
       <c r="A324" s="0" t="s">
-        <v>692</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="325">
       <c r="A325" s="0" t="s">
-        <v>693</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="326">
       <c r="A326" s="0" t="s">
-        <v>694</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="0" t="s">
-        <v>695</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="328">
       <c r="A328" s="0" t="s">
-        <v>696</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="329">
       <c r="A329" s="0" t="s">
-        <v>697</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="330">
       <c r="A330" s="0" t="s">
-        <v>698</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="331">
       <c r="A331" s="0" t="s">
-        <v>699</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="332">
       <c r="A332" s="0" t="s">
-        <v>700</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="333">
       <c r="A333" s="0" t="s">
-        <v>701</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="334">
       <c r="A334" s="0" t="s">
-        <v>702</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="335">
       <c r="A335" s="0" t="s">
-        <v>703</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="336">
       <c r="A336" s="0" t="s">
-        <v>704</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="337">
       <c r="A337" s="0" t="s">
-        <v>705</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="338">
       <c r="A338" s="0" t="s">
-        <v>706</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="339">
       <c r="A339" s="0" t="s">
-        <v>707</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="340">
       <c r="A340" s="0" t="s">
-        <v>708</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="341">
       <c r="A341" s="0" t="s">
-        <v>709</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="342">
       <c r="A342" s="0" t="s">
-        <v>710</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="343">
       <c r="A343" s="0" t="s">
-        <v>711</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="344">
       <c r="A344" s="0" t="s">
-        <v>712</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="345">
       <c r="A345" s="0" t="s">
-        <v>713</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="346">
       <c r="A346" s="0" t="s">
-        <v>714</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="347">
       <c r="A347" s="0" t="s">
-        <v>715</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="348">
       <c r="A348" s="0" t="s">
-        <v>716</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="349">
       <c r="A349" s="0" t="s">
-        <v>717</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="350">
       <c r="A350" s="0" t="s">
-        <v>718</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="351">
       <c r="A351" s="0" t="s">
-        <v>719</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="352">
       <c r="A352" s="0" t="s">
-        <v>720</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="353">
       <c r="A353" s="0" t="s">
-        <v>721</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="354">
       <c r="A354" s="0" t="s">
-        <v>722</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="355">
       <c r="A355" s="0" t="s">
-        <v>723</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="356">
       <c r="A356" s="0" t="s">
-        <v>724</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="357">
       <c r="A357" s="0" t="s">
-        <v>725</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="358">
       <c r="A358" s="0" t="s">
-        <v>726</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="359">
       <c r="A359" s="0" t="s">
-        <v>727</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="360">
       <c r="A360" s="0" t="s">
-        <v>728</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="361">
       <c r="A361" s="0" t="s">
-        <v>729</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="362">
       <c r="A362" s="0" t="s">
-        <v>730</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="363">
       <c r="A363" s="0" t="s">
-        <v>731</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="364">
       <c r="A364" s="0" t="s">
-        <v>732</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="365">
       <c r="A365" s="0" t="s">
-        <v>733</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="366">
       <c r="A366" s="0" t="s">
-        <v>734</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="367">
       <c r="A367" s="0" t="s">
-        <v>735</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="368">
       <c r="A368" s="0" t="s">
-        <v>736</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="369">
       <c r="A369" s="0" t="s">
-        <v>737</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="370">
       <c r="A370" s="0" t="s">
-        <v>738</v>
+        <v>1108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>